<commit_message>
evaluated cypress for test and reporting with cucumber.
</commit_message>
<xml_diff>
--- a/docs/compare-tech.xlsx
+++ b/docs/compare-tech.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/trigunams/Workspace/compare-ui-automation-frameworks/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE3BB04-6281-F646-8344-1255279D088A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61469EC6-61B5-7542-9AEE-00BDCB2B292F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{F8CF246C-FACE-D746-AA8D-914FE7E05013}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>Criteria</t>
   </si>
@@ -61,9 +61,6 @@
     <t>Puppeteer</t>
   </si>
   <si>
-    <t>Migrating from Protractor to Cypress</t>
-  </si>
-  <si>
     <t>Migration from Protractor</t>
   </si>
   <si>
@@ -127,9 +124,6 @@
     <t>Not by default</t>
   </si>
   <si>
-    <t>config.json</t>
-  </si>
-  <si>
     <t>Available</t>
   </si>
   <si>
@@ -149,6 +143,40 @@
   </si>
   <si>
     <t>W3C Recommended, Open Source</t>
+  </si>
+  <si>
+    <t>Migrating from Protractor to Cypress
+Co-exist and manual</t>
+  </si>
+  <si>
+    <t>BDD</t>
+  </si>
+  <si>
+    <t>Supports Cucumber based testing using .feature files</t>
+  </si>
+  <si>
+    <t>None?</t>
+  </si>
+  <si>
+    <t>config/app.config.json</t>
+  </si>
+  <si>
+    <t>Yes, bit tricky but after first few attempts its easy.</t>
+  </si>
+  <si>
+    <t>Yes a video is automaticlly created for every feature.</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>There are no hard dependencies</t>
+  </si>
+  <si>
+    <t>Yes with the preprocessor.</t>
+  </si>
+  <si>
+    <t>Yes available to generate json report.</t>
   </si>
 </sst>
 </file>
@@ -180,12 +208,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -201,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -212,14 +246,17 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -536,10 +573,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D4BCA43-FA87-124A-B2FB-50B5F9CF5CB6}">
-  <dimension ref="C2:K11"/>
+  <dimension ref="C2:K12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2:K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -549,7 +588,7 @@
     <col min="4" max="4" width="28.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.5" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
@@ -558,19 +597,19 @@
   </cols>
   <sheetData>
     <row r="2" spans="3:11" x14ac:dyDescent="0.2">
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+    </row>
+    <row r="3" spans="3:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="C3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-    </row>
-    <row r="3" spans="3:11" ht="17" x14ac:dyDescent="0.2">
-      <c r="C3" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>0</v>
@@ -581,52 +620,52 @@
       <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="6" t="s">
         <v>4</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="3:11" s="4" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="C4" s="4" t="s">
+    <row r="4" spans="3:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="E4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="3:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="F4" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="3:11" ht="68" x14ac:dyDescent="0.2">
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
@@ -634,92 +673,121 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>8</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="3:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="3:11" ht="34" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+      <c r="G6" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="3:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C7" s="5"/>
       <c r="D7" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="3:11" ht="51" x14ac:dyDescent="0.2">
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="3:11" ht="68" x14ac:dyDescent="0.2">
       <c r="C9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="3:11" ht="68" x14ac:dyDescent="0.2">
       <c r="C10" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="3:11" ht="51" x14ac:dyDescent="0.2">
+      <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="3:11" ht="34" x14ac:dyDescent="0.2">
-      <c r="C11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>26</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="3:11" ht="34" x14ac:dyDescent="0.2">
+      <c r="C12" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -728,7 +796,7 @@
     <mergeCell ref="C6:C7"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G5" r:id="rId1" location="Introduction" xr:uid="{6610253D-E0A8-4749-9309-496A748CAADA}"/>
+    <hyperlink ref="G5" r:id="rId1" location="Introduction" display="Migrating from Protractor to Cypress" xr:uid="{6610253D-E0A8-4749-9309-496A748CAADA}"/>
     <hyperlink ref="K5" r:id="rId2" xr:uid="{FA12CD0B-99F4-464A-BA31-0E5823BF7BA3}"/>
     <hyperlink ref="E3" r:id="rId3" location="/infrastructure" xr:uid="{1FA9A5E1-1A71-C845-A4FA-5AD3F5261A0F}"/>
     <hyperlink ref="F3" r:id="rId4" xr:uid="{EDF6F316-9E41-5642-945F-D6C8732642A5}"/>

</xml_diff>